<commit_message>
Updated BOM with major components.
I also added all appropriate data sheets to the data sheets folder.
</commit_message>
<xml_diff>
--- a/411 Project/nocLock/BOMs/Knock Lock BOM.xlsx
+++ b/411 Project/nocLock/BOMs/Knock Lock BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="000 Level" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>PWA Level</t>
   </si>
@@ -73,19 +73,68 @@
     <t>Batteries</t>
   </si>
   <si>
-    <t>ATmega88A</t>
+    <t>5V Voltage regulator</t>
+  </si>
+  <si>
+    <t>UA78M05CDCYR</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>Schmitt Trigger</t>
+  </si>
+  <si>
+    <t>SN74HC14DR</t>
+  </si>
+  <si>
+    <t>NMOS Transistors</t>
+  </si>
+  <si>
+    <t>DMN63D8LDW-7</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Bi-Color LED</t>
+  </si>
+  <si>
+    <t>WP59SURKSGW</t>
+  </si>
+  <si>
+    <t>Common Anode</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>ATMEGA88A-AUR</t>
+  </si>
+  <si>
+    <t>Piezo buzzer</t>
+  </si>
+  <si>
+    <t>CEP-1110</t>
+  </si>
+  <si>
+    <t>Darlington Pair</t>
+  </si>
+  <si>
+    <t>FZT605TA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -102,6 +151,29 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,17 +230,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,31 +611,235 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="23">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.72</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -588,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -870,6 +1159,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added more datasheets and updated BOM
</commit_message>
<xml_diff>
--- a/411 Project/nocLock/BOMs/Knock Lock BOM.xlsx
+++ b/411 Project/nocLock/BOMs/Knock Lock BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="000 Level" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>PWA Level</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>FZT605TA</t>
+  </si>
+  <si>
+    <t>PJ-065B</t>
+  </si>
+  <si>
+    <t>Barrel Jack</t>
   </si>
 </sst>
 </file>
@@ -613,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -852,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -877,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -955,15 +961,20 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.58</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>

</xml_diff>